<commit_message>
Entrega final Reto 3
</commit_message>
<xml_diff>
--- a/Docs/Tablas.xlsx
+++ b/Docs/Tablas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1902876135bf28ab/Documents/EDA/Reto 3/Reto3-G4/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3282A73F-5B40-4922-9D79-C8646E5348FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{3282A73F-5B40-4922-9D79-C8646E5348FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{1180F07A-E9C4-431E-9411-4A1DDEFD50AA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView minimized="1" xWindow="14268" yWindow="3048" windowWidth="15360" windowHeight="7812" firstSheet="4" activeTab="6" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +162,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Dax-Regular"/>
     </font>
   </fonts>
   <fills count="3">
@@ -179,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,11 +217,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -250,11 +269,63 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="36">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Dax-Regular"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1162,46 +1233,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Dax-Regular"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1606,7 +1637,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1664,51 +1695,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -1793,6 +1779,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1800,8 +1795,17 @@
             <c:numRef>
               <c:f>Datos!$B$15:$B$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>61.734000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>242.18199999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>414.27100000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1900,7 +1904,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1938,7 +1942,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2017,7 +2021,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2055,7 +2059,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2097,7 +2101,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2134,7 +2138,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2210,7 +2214,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2258,56 +2262,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2371,56 +2340,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$20:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2428,8 +2362,17 @@
             <c:numRef>
               <c:f>Datos!$F$20:$F$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2651.7640000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3972.6149999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4155.7439999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2556,7 +2499,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2594,7 +2537,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2678,7 +2621,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2716,7 +2659,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2758,7 +2701,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2795,7 +2738,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2871,7 +2814,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2929,50 +2872,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -3051,56 +2950,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3108,8 +2972,17 @@
             <c:numRef>
               <c:f>Datos!$G$15:$G$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>38441.610999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>511123.85600000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1637760.284</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3208,7 +3081,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3246,7 +3119,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3325,7 +3198,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3363,7 +3236,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3405,7 +3278,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3442,7 +3315,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3518,7 +3391,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3566,56 +3439,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3679,56 +3517,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$20:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3736,8 +3539,17 @@
             <c:numRef>
               <c:f>Datos!$G$20:$G$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>299144.38500000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>333723.48499999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6517063.8559999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3864,7 +3676,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3902,7 +3714,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3986,7 +3798,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4024,7 +3836,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4066,7 +3878,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4103,7 +3915,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4189,7 +4001,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4247,57 +4059,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4367,6 +4143,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4374,8 +4159,17 @@
             <c:numRef>
               <c:f>Datos!$B$20:$B$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>21.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4474,7 +4268,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4512,7 +4306,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4599,7 +4393,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4637,7 +4431,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4679,7 +4473,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4716,7 +4510,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4802,7 +4596,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4850,50 +4644,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -4978,6 +4728,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4985,8 +4744,17 @@
             <c:numRef>
               <c:f>Datos!$C$15:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.861000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>133.84899999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>277.96100000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5113,7 +4881,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5151,7 +4919,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5230,7 +4998,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5268,7 +5036,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -5310,7 +5078,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5347,7 +5115,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5433,7 +5201,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5481,56 +5249,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5600,6 +5333,15 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5607,8 +5349,17 @@
             <c:numRef>
               <c:f>Datos!$C$20:$C$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>30.672000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.07</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5707,7 +5458,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5745,7 +5496,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -5884,7 +5635,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5922,7 +5673,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -5964,7 +5715,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6001,7 +5752,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6081,7 +5832,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6139,50 +5890,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -6261,56 +5968,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6318,8 +5990,17 @@
             <c:numRef>
               <c:f>Datos!$D$15:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13.452</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.811000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130.059</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6473,7 +6154,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6511,7 +6192,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -6590,7 +6271,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6628,7 +6309,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -6670,7 +6351,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6707,7 +6388,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6783,7 +6464,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6841,56 +6522,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6954,56 +6600,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$20:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7011,8 +6622,17 @@
             <c:numRef>
               <c:f>Datos!$D$20:$D$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>14.852</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.155999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.68</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7166,7 +6786,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7204,7 +6824,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -7288,7 +6908,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7326,7 +6946,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -7368,7 +6988,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7405,7 +7025,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7486,7 +7106,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7534,50 +7154,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -7656,56 +7232,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7713,8 +7254,17 @@
             <c:numRef>
               <c:f>Datos!$E$15:$E$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>611.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4082.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4805.5249999999996</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7813,7 +7363,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7851,7 +7401,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -7930,7 +7480,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7968,7 +7518,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -8010,7 +7560,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8047,7 +7597,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8123,7 +7673,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8171,56 +7721,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$7:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8284,56 +7799,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$20:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8341,8 +7821,17 @@
             <c:numRef>
               <c:f>Datos!$E$20:$E$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2570.5070000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5001.8040000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5619.3270000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -8441,7 +7930,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8479,7 +7968,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -8563,7 +8052,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8601,7 +8090,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -8643,7 +8132,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -8680,7 +8169,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8756,7 +8245,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8804,50 +8293,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$2:$A$4</c:f>
@@ -8926,56 +8371,21 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Datos!$A$15:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8983,8 +8393,17 @@
             <c:numRef>
               <c:f>Datos!$F$15:$F$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7750.09</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30949.489000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132028.60800000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -9083,7 +8502,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9121,7 +8540,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -9200,7 +8619,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9238,7 +8657,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -9280,7 +8699,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9317,7 +8736,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16308,8 +15727,8 @@
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659906" cy="6284259"/>
+    <xdr:pos x="0" y="1089660"/>
+    <xdr:ext cx="6957060" cy="4899660"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -16336,8 +15755,8 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
   <xdr:absoluteAnchor>
-    <xdr:pos x="8694420" y="0"/>
-    <xdr:ext cx="8659906" cy="6284259"/>
+    <xdr:pos x="7383780" y="1219200"/>
+    <xdr:ext cx="6564406" cy="4379259"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 1">
@@ -16386,52 +15805,52 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D22C05A1-E12C-4199-9FB6-5E4FBB74E4CE}" name="Table16" displayName="Table16" ref="A6:G9" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A6:G9" xr:uid="{2C2BC8F6-7973-4113-AD2A-A5438FE4F598}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F51D620E-F6AB-4198-854E-1DBC011ED1C9}" name="Maquina 1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{771A8AF9-02A9-40D1-B684-060654790566}" name="Req 1 Memoria M1" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{3648047C-FCA2-4CBF-930D-171D858BB23E}" name="Req 2 Memoria M1" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{ABCB9616-BC98-4F26-8570-A123C8449050}" name="Req 3 Memoria M1" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{354C7E6A-9D9B-435F-84CF-21D5B417D4B8}" name="Req 4 Memoria M1" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{B08087E7-A097-4B94-9A63-1EAEE355B242}" name="Req 5 Memoria M1" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{0A9BE0C8-A628-46E6-9976-E59CA7C7D4D6}" name="Carga M1" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{F51D620E-F6AB-4198-854E-1DBC011ED1C9}" name="Maquina 1" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{771A8AF9-02A9-40D1-B684-060654790566}" name="Req 1 Memoria M1" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{3648047C-FCA2-4CBF-930D-171D858BB23E}" name="Req 2 Memoria M1" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{ABCB9616-BC98-4F26-8570-A123C8449050}" name="Req 3 Memoria M1" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{354C7E6A-9D9B-435F-84CF-21D5B417D4B8}" name="Req 4 Memoria M1" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{B08087E7-A097-4B94-9A63-1EAEE355B242}" name="Req 5 Memoria M1" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{0A9BE0C8-A628-46E6-9976-E59CA7C7D4D6}" name="Carga M1" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{59945499-AB99-4BA5-8DF5-97B49CC49E63}" name="Table17" displayName="Table17" ref="A14:G17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A14:G17" xr:uid="{B8C754A0-67D4-4B43-86DC-D904E0737C4B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{04488F60-343A-4C83-B16E-0A10442D5404}" name="Table173" displayName="Table173" ref="A14:G18" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A14:G18" xr:uid="{C5C4AD15-0599-4463-8F18-752225F8FBCD}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A9D6E7C5-7068-4FB8-98EF-04B0E7F0A8D8}" name="Maquina 2" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{D2842BBF-4594-4F7B-AB04-9CD434602D29}" name="Req 1 Tiempo M2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{765E61D4-A10E-4306-A150-0B79894FAE80}" name="Req 2 Tiempo M2" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{B95A2C9A-4724-4E62-95E6-3078AF5CC00B}" name="Req 3 Tiempo M2" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{912350D6-EACC-4109-894A-0EFCA0DE432F}" name="Req 4 Tiempo M2" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{7F05FC75-B46E-4CDB-A2C2-4FFED58D66EA}" name="Req 5 Tiempo M2" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{92559E6F-C83F-4764-8519-43B442240B8D}" name="Carga M2" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{962B08B9-55D4-4C7F-A04E-BECD3D5766EA}" name="Maquina 2" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{EA3D047E-35BE-421E-8BE7-D06D2A1434A8}" name="Req 1 Tiempo M2" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{F82825E4-ECCA-43DE-94B7-EDF53961C4DC}" name="Req 2 Tiempo M2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{C44843F5-B981-4458-907B-C6D606B44810}" name="Req 3 Tiempo M2" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{EB629C40-ABED-4767-8067-C031A753C8AC}" name="Req 4 Tiempo M2" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{71B96266-F0B5-4D9C-A6EF-90251067CC27}" name="Req 5 Tiempo M2" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{BDB8DAFB-4FAE-4734-801C-DEEED3414A0C}" name="Carga M2" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C876BE91-63D9-4735-9B67-B8DD17C7B2DA}" name="Table18" displayName="Table18" ref="A19:G22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A19:G22" xr:uid="{12A1EBE4-5411-4018-BF18-3FEF79EA825C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EFDBE6F1-8C42-479C-B943-8881954298CF}" name="Table184" displayName="Table184" ref="A19:G22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A19:G22" xr:uid="{2B190FF8-C70F-4780-A0BF-3CF6E744E763}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A268468E-64F4-4D45-80A8-688751D35AC9}" name="Maquina 2" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C56B6F3A-B572-4079-B3F3-899B31D72DCD}" name="Req 1 Memoria M2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{0DEC6835-DE5D-4750-B0C6-12C8E8ACBA4B}" name="Req 2 Memoria M2" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6A96B2D4-78EB-4A01-9C5B-2E6EE704775B}" name="Req 3 Memoria M2" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FA5B4EC9-2611-4919-B1B2-E16FDF977B2C}" name="Req 4 Memoria M2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{3BC1DDEC-D62C-484C-B414-290E541C1FC5}" name="Req 5 Memoria M2" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A9B3E79C-8FC2-4C9F-88AF-7C3244DD0045}" name="Carga M2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A3054EE5-5B86-4145-A597-E652C0729F84}" name="Maquina 2" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6AF8647D-0159-42AA-A7D5-4A2E505615EE}" name="Req 1 Memoria M2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{839EAF35-C53D-4E4F-9267-AA7F71779346}" name="Req 2 Memoria M2" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{F5FB5CFA-EFC9-4F88-98E1-CAE05E887435}" name="Req 3 Memoria M2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{907BE8BC-555A-4614-95A6-BC8B82C0435B}" name="Req 4 Memoria M2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{25540B12-F6EE-4AC7-84A7-4FA7865F68DB}" name="Req 5 Memoria M2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{30A00E05-8BFF-411E-98A6-D6A37D77EF1B}" name="Carga M2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -16729,17 +16148,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16766,7 +16185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -16789,7 +16208,7 @@
         <v>63172</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7">
       <c r="A3" s="10">
         <v>5</v>
       </c>
@@ -16812,7 +16231,7 @@
         <v>114192.273</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7">
       <c r="A4" s="10">
         <v>10</v>
       </c>
@@ -16831,7 +16250,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="27.6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -16854,8 +16273,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:7">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
       <c r="B7" s="11">
         <v>21.398</v>
       </c>
@@ -16875,8 +16296,10 @@
         <v>299143.35399999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
       <c r="B8" s="11">
         <v>21.398</v>
       </c>
@@ -16897,7 +16320,9 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10">
+        <v>10</v>
+      </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -16934,110 +16359,197 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="9">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11">
+        <v>61.734000000000002</v>
+      </c>
+      <c r="C15" s="11">
+        <v>10.861000000000001</v>
+      </c>
+      <c r="D15" s="11">
+        <v>13.452</v>
+      </c>
+      <c r="E15" s="11">
+        <v>611.75</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7750.09</v>
+      </c>
+      <c r="G15" s="11">
+        <v>38441.610999999997</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="A16" s="9">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11">
+        <v>242.18199999999999</v>
+      </c>
+      <c r="C16" s="11">
+        <v>133.84899999999999</v>
+      </c>
+      <c r="D16" s="11">
+        <v>94.811000000000007</v>
+      </c>
+      <c r="E16" s="11">
+        <v>4082.07</v>
+      </c>
+      <c r="F16" s="11">
+        <v>30949.489000000001</v>
+      </c>
+      <c r="G16" s="11">
+        <v>511123.85600000003</v>
+      </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="A17" s="9">
+        <v>10</v>
+      </c>
+      <c r="B17" s="11">
+        <v>414.27100000000002</v>
+      </c>
+      <c r="C17" s="11">
+        <v>277.96100000000001</v>
+      </c>
+      <c r="D17" s="11">
+        <v>130.059</v>
+      </c>
+      <c r="E17" s="11">
+        <v>4805.5249999999996</v>
+      </c>
+      <c r="F17" s="11">
+        <v>132028.60800000001</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1637760.284</v>
+      </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:7" ht="27.6">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="A20" s="9">
+        <v>1</v>
+      </c>
+      <c r="B20" s="11">
+        <v>21.875</v>
+      </c>
+      <c r="C20" s="11">
+        <v>30.672000000000001</v>
+      </c>
+      <c r="D20" s="11">
+        <v>14.852</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2570.5070000000001</v>
+      </c>
+      <c r="F20" s="11">
+        <v>2651.7640000000001</v>
+      </c>
+      <c r="G20" s="11">
+        <v>299144.38500000001</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="9">
+        <v>5</v>
+      </c>
+      <c r="B21" s="11">
+        <v>21.398</v>
+      </c>
+      <c r="C21" s="11">
+        <v>29.555</v>
+      </c>
+      <c r="D21" s="11">
+        <v>16.155999999999999</v>
+      </c>
+      <c r="E21" s="11">
+        <v>5001.8040000000001</v>
+      </c>
+      <c r="F21" s="11">
+        <v>3972.6149999999998</v>
+      </c>
+      <c r="G21" s="11">
+        <v>333723.48499999999</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="A22" s="9">
+        <v>10</v>
+      </c>
+      <c r="B22" s="11">
+        <v>21.305</v>
+      </c>
+      <c r="C22" s="11">
+        <v>31.07</v>
+      </c>
+      <c r="D22" s="11">
+        <v>16.68</v>
+      </c>
+      <c r="E22" s="11">
+        <v>5619.3270000000002</v>
+      </c>
+      <c r="F22" s="11">
+        <v>4155.7439999999997</v>
+      </c>
+      <c r="G22" s="11">
+        <v>6517063.8559999997</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23"/>
@@ -17073,11 +16585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05A2A40-DA18-42A6-B50B-58E51A67EFC5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="E4" workbookViewId="0">
       <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17088,11 +16600,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17735EF2-994E-46E5-9B13-718EE674823D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17103,11 +16615,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB2D21DE-7039-49F7-9ED1-F058A486C07D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17118,11 +16630,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B6771B-C785-4E97-A481-D6121A6CC38F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17137,7 +16649,7 @@
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17148,11 +16660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C798315-EAB6-451A-AF78-BA9AB83D8339}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -17166,15 +16678,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -17385,14 +16888,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>